<commit_message>
included parameters & randomized order
</commit_message>
<xml_diff>
--- a/pilot_Test/static/Parameters.xlsx
+++ b/pilot_Test/static/Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frauke/GithubRepoTree/pilot_Test/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37B9EE89-574C-3C45-803B-A8AEC0B7C1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC0F601-F931-2B40-9EFD-4904AB556BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{28A043C9-DE9F-A64A-A4AD-251F26E254DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{28A043C9-DE9F-A64A-A4AD-251F26E254DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>num_x_A</t>
   </si>
   <si>
-    <t>image_title_1</t>
-  </si>
-  <si>
     <t>num_x_B</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>matrix_290.png</t>
+  </si>
+  <si>
+    <t>image_title_B</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,21 +455,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>330</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>70</v>
@@ -477,13 +477,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>310</v>
@@ -491,13 +491,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>110</v>
@@ -505,13 +505,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>300</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>320</v>
@@ -519,13 +519,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>280</v>
@@ -533,13 +533,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>270</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>100</v>
@@ -547,13 +547,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>290</v>

</xml_diff>